<commit_message>
Cambio de lugar de evalucaion de las estrategias
</commit_message>
<xml_diff>
--- a/EmotionRegulation/EmotionRegulationAsset/Conscientiousness.xlsx
+++ b/EmotionRegulation/EmotionRegulationAsset/Conscientiousness.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R0d9da18c0b6a4074"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rcfa2ddbc5c204ba3"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t xml:space="preserve">MOOD     </x:t>
   </x:si>
@@ -41,7 +41,7 @@
     <x:t>--</x:t>
   </x:si>
   <x:si>
-    <x:t>Not-Enter</x:t>
+    <x:t>Not-Talk</x:t>
   </x:si>
   <x:si>
     <x:t>Situation Selection</x:t>
@@ -83,9 +83,6 @@
     <x:t>Fired</x:t>
   </x:si>
   <x:si>
-    <x:t>Attention Deployment</x:t>
-  </x:si>
-  <x:si>
     <x:t>Crash</x:t>
   </x:si>
   <x:si>
@@ -101,7 +98,7 @@
     <x:t>Low Neuroticism</x:t>
   </x:si>
   <x:si>
-    <x:t>Middle Agreeableness</x:t>
+    <x:t>Low Agreeableness</x:t>
   </x:si>
   <x:si>
     <x:t>Low Openness</x:t>
@@ -498,13 +495,13 @@
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>0</x:v>
+        <x:v>0.6227638125419617</x:v>
       </x:c>
       <x:c r="B3" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>1.3367782831192017</x:v>
+        <x:v>2.005167245864868</x:v>
       </x:c>
       <x:c r="D3" t="s">
         <x:v>12</x:v>
@@ -515,13 +512,13 @@
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>0.8303518295288086</x:v>
+        <x:v>1.501367449760437</x:v>
       </x:c>
       <x:c r="B4" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>2.6735565662384033</x:v>
+        <x:v>2.8519487380981445</x:v>
       </x:c>
       <x:c r="D4" t="s">
         <x:v>14</x:v>
@@ -532,13 +529,13 @@
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>2.3478033542633057</x:v>
+        <x:v>3.0708096027374268</x:v>
       </x:c>
       <x:c r="B5" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>4.9165802001953125</x:v>
+        <x:v>5.108794689178467</x:v>
       </x:c>
       <x:c r="D5" t="s">
         <x:v>15</x:v>
@@ -549,13 +546,13 @@
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>2.5297117233276367</x:v>
+        <x:v>3.308736801147461</x:v>
       </x:c>
       <x:c r="B6" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>0.672534167766571</x:v>
+        <x:v>0.879641056060791</x:v>
       </x:c>
       <x:c r="D6" t="s">
         <x:v>17</x:v>
@@ -566,13 +563,13 @@
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>3.3188230991363525</x:v>
+        <x:v>4.158206939697266</x:v>
       </x:c>
       <x:c r="B7" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>2.6343255043029785</x:v>
+        <x:v>2.8574790954589844</x:v>
       </x:c>
       <x:c r="D7" t="s">
         <x:v>18</x:v>
@@ -583,13 +580,13 @@
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>3.280703067779541</x:v>
+        <x:v>4.110445976257324</x:v>
       </x:c>
       <x:c r="B8" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>2.5153634548187256</x:v>
+        <x:v>2.7284398078918457</x:v>
       </x:c>
       <x:c r="D8" t="s">
         <x:v>19</x:v>
@@ -600,33 +597,33 @@
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>2.325873851776123</x:v>
+        <x:v>2.97580885887146</x:v>
       </x:c>
       <x:c r="B9" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>2.9530186653137207</x:v>
+        <x:v>3.5012764930725098</x:v>
       </x:c>
       <x:c r="D9" t="s">
         <x:v>22</x:v>
       </x:c>
       <x:c r="E9" t="s">
-        <x:v>23</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>0.6377917528152466</x:v>
+        <x:v>1.3380838632583618</x:v>
       </x:c>
       <x:c r="B10" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>5.349249839782715</x:v>
+        <x:v>5.163074016571045</x:v>
       </x:c>
       <x:c r="D10" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E10" t="s">
         <x:v>13</x:v>
@@ -634,16 +631,16 @@
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>3.0596415996551514</x:v>
+        <x:v>3.814192771911621</x:v>
       </x:c>
       <x:c r="B11" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>7.821430206298828</x:v>
+        <x:v>8.0220308303833</x:v>
       </x:c>
       <x:c r="D11" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E11" t="s">
         <x:v>13</x:v>
@@ -651,47 +648,47 @@
     </x:row>
     <x:row r="12">
       <x:c r="F12" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="F13" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="F14" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="F15" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="F16" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="G17" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="G18" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="G19" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="H20" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>